<commit_message>
Correction noms Organization (#290)
* Correction cardinalités noms orga

* Amélioration descriptions noms orga

* Modification cardinalité Organization.name f25d7c1dc4cfcfc972ecda860f7b7e57e6d95be3
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-ror-organization.xlsx
+++ b/main/ig/StructureDefinition-ror-organization.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-16T09:35:34+00:00</t>
+    <t>2024-02-16T16:20:17+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1770,9 +1770,7 @@
     <t>Organization.name</t>
   </si>
   <si>
-    <t>raisonSociale (EJ) : Raison sociale complète de l'entité juridique
-ou nom de l'EG :  Nom sous lequel l'entité géographique exerce son activité
-ou nom de l'OI : Nom de l'organisation interne</t>
+    <t>raisonSociale (EJ) ou denominationEG (EG) ou nomOI (OI) - Remarque : Décalage provisoire de la cardinalité par rapport au modèle d'exposition (1..1)</t>
   </si>
   <si>
     <t>A name associated with the organization.</t>
@@ -1800,7 +1798,7 @@
 </t>
   </si>
   <si>
-    <t>complementRaisonSociale (EJ) : Suite de la raison sociale, si elle existe</t>
+    <t>complementRaisonSociale (EJ) ou complementDenominationEG (EG)</t>
   </si>
   <si>
     <t>Extension créée dans le cadre du ROR pour nom complémentaire de l'EJ (complementRaisonSociale)  ou nom complémentaire de l'EG (DenominationEG)</t>
@@ -1821,7 +1819,7 @@
     <t>Organization.alias</t>
   </si>
   <si>
-    <t>nom opérationnel (EG) : l’appellation communément utilisée par les acteurs de santé pour désigner l'entité géographique</t>
+    <t>nomOperationnel (EG) : l’appellation communément utilisée par les acteurs de santé pour désigner l'entité géographique</t>
   </si>
   <si>
     <t>A list of alternate names that the organization is known as, or was known as in the past.</t>
@@ -19313,7 +19311,7 @@
         <v>80</v>
       </c>
       <c r="H157" t="s" s="2">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="I157" t="s" s="2">
         <v>72</v>
@@ -19510,7 +19508,7 @@
         <v>73</v>
       </c>
       <c r="G159" t="s" s="2">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="H159" t="s" s="2">
         <v>81</v>

</xml_diff>

<commit_message>
consigne de fiche de saisie (#265)
* 1st iteration

* 2 eme itération

* 1st iteration example

* corrections example

* example 2nd iteration

* iteration 3 exemple b4e4c0dc78fe532f6861d171a8c0fa02fdef81f8
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-ror-organization.xlsx
+++ b/main/ig/StructureDefinition-ror-organization.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-13T16:38:24+00:00</t>
+    <t>2024-03-13T17:00:38+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1316,7 +1316,7 @@
   <si>
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
   &lt;coding&gt;
-    &lt;system value="https://mos.esante.gouv.fr/NOS/TRE_R345-TypeIdentifiantAutre/FHIR/TRE-R345-TypeIdentifiantAutre"/&gt;
+    &lt;system value="https://mos.esante.gouv.fr/NOS/TRE_R345-TypeIdentifiantAutre/FHIR/TRE_R345-TypeIdentifiantAutre"/&gt;
     &lt;code value="42"/&gt;
   &lt;/coding&gt;
 &lt;/valueCodeableConcept&gt;</t>

</xml_diff>

<commit_message>
Sd update system identifier orga (#349)
* ajout https

* https sirene f044bce58d4a47fe5a90eb7de85c934d503be894
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-ror-organization.xlsx
+++ b/main/ig/StructureDefinition-ror-organization.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-04-11T09:28:17+00:00</t>
+    <t>2024-04-11T09:33:38+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1149,7 +1149,7 @@
     <t>Organization.identifier:finess.system</t>
   </si>
   <si>
-    <t>http://finess.esante.gouv.fr</t>
+    <t>https://finess.esante.gouv.fr</t>
   </si>
   <si>
     <t>Organization.identifier:finess.value</t>
@@ -1193,7 +1193,7 @@
     <t>Organization.identifier:sirene.system</t>
   </si>
   <si>
-    <t>http://sirene.fr</t>
+    <t>https://sirene.fr</t>
   </si>
   <si>
     <t>Organization.identifier:sirene.value</t>
@@ -1237,7 +1237,7 @@
     <t>Organization.identifier:rppsRang.system</t>
   </si>
   <si>
-    <t>http://rppsrang.esante.gouv.fr</t>
+    <t>https://rppsrang.esante.gouv.fr</t>
   </si>
   <si>
     <t>Organization.identifier:rppsRang.value</t>
@@ -1366,7 +1366,7 @@
     <t>Organization.identifier:adeliRang.system</t>
   </si>
   <si>
-    <t>http://adelirang.esante.gouv.fr</t>
+    <t>https://adelirang.esante.gouv.fr</t>
   </si>
   <si>
     <t>Organization.identifier:adeliRang.value</t>

</xml_diff>

<commit_message>
Correction définition type fermeture (#353)
* Correction définition type fermeture

* Update README.md

* Create a_tests_githubPages.yml

---------

Co-authored-by: sly-kereval <125375447+sly-kereval@users.noreply.github.com>
Co-authored-by: Mael PRIOUR <101335975+M-Priour@users.noreply.github.com> f8b83b97be8b40412880235131d0efcea109990b
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-ror-organization.xlsx
+++ b/main/ig/StructureDefinition-ror-organization.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-05-03T15:00:21+00:00</t>
+    <t>2024-05-13T08:42:46+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -794,7 +794,7 @@
 </t>
   </si>
   <si>
-    <t>datePrevisionnelleReouverture (OI)</t>
+    <t>datePrevisionnelleReouverture (OI) : Date prévisionnelle à partir de laquelle la prestation sera de nouveau assurée</t>
   </si>
   <si>
     <t>Extension créée dans le cadre du ROR pour définir la date prévisionnelle de réouverture de l'organisation interne.</t>
@@ -826,7 +826,7 @@
 </t>
   </si>
   <si>
-    <t>typeFermeture (EJ + EG + OI) : Date prévisionnelle à partir de laquelle la prestation sera de nouveau assurée</t>
+    <t>typeFermeture (EJ + EG + OI) : Le type de fermeture d'un niveau organisationnel indique la temporalité de la fermeture.</t>
   </si>
   <si>
     <t>Extension créée dans le cadre du ROR pour définir le type de fermeture de l'organisation.</t>

</xml_diff>

<commit_message>
intégration specs fonc de consignes fiche de saisie (#365) 5beeea5e154f2b98e8588e0792ea038a4c00ab8e
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-ror-organization.xlsx
+++ b/main/ig/StructureDefinition-ror-organization.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-05-23T14:57:06+00:00</t>
+    <t>2024-07-02T15:46:36+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -2237,7 +2237,7 @@
   </si>
   <si>
     <t>base64Binary
-booleancanonicalcodedatedateTimedecimalidinstantintegerinteger64markdownoidpositiveIntstringtimeunsignedInturiurluuidAddressAgeAnnotationAttachmentCodeableConceptCodeableReferenceCodingContactPointCountDistanceDurationHumanNameIdentifierMoneyPeriodQuantityRangeRatioRatioRangeReferenceSampledDataSignatureTimingContactDetailDataRequirementExpressionParameterDefinitionRelatedArtifactTriggerDefinitionUsageContextAvailabilityExtendedContactDetailDosageMeta</t>
+booleancanonicalcodedatedateTimedecimalidinstantintegermarkdownoidpositiveIntstringtimeunsignedInturiurluuidAddressAgeAnnotationAttachmentCodeableConceptCodingContactPointCountDistanceDurationHumanNameIdentifierMoneyPeriodQuantityRangeRatioReferenceSampledDataSignatureTimingContactDetailDataRequirementExpressionParameterDefinitionRelatedArtifactTriggerDefinitionUsageContextDosageMeta</t>
   </si>
   <si>
     <t>Organization.address.use</t>

</xml_diff>

<commit_message>
Fix short Organization.extension:organization-period (#426)
Dans le MEV3 la dateOuverture ne concerne pas l'EJ mais l'EG et l'OI 6ed443c80bd89c7e43f1f3e63894b60a8739a768
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-ror-organization.xlsx
+++ b/main/ig/StructureDefinition-ror-organization.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-17T14:29:52+00:00</t>
+    <t>2025-07-17T15:27:59+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -838,7 +838,7 @@
     <t>organization-period</t>
   </si>
   <si>
-    <t>dateOuverture (EJ + OI) + dateFermeture (EJ + EG + OI)</t>
+    <t>dateOuverture (EG + OI) + dateFermeture (EJ + EG + OI)</t>
   </si>
   <si>
     <t>Organization.extension:ror-meta-comment</t>

</xml_diff>